<commit_message>
Read only view of the key value pairs in the item view
</commit_message>
<xml_diff>
--- a/internewshid/chn_spreadsheet/tests/test_files/sample_kobo_keyValues.xlsx
+++ b/internewshid/chn_spreadsheet/tests/test_files/sample_kobo_keyValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -70,6 +70,33 @@
     <t xml:space="preserve">KV1</t>
   </si>
   <si>
+    <t xml:space="preserve">KV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KV10</t>
+  </si>
+  <si>
     <t xml:space="preserve">2018-08-09T12:14:26.766+06</t>
   </si>
   <si>
@@ -107,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two</t>
   </si>
   <si>
     <t xml:space="preserve">2018-08-19T13:01:27.511+06</t>
@@ -148,7 +178,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">tes </t>
     </r>
@@ -158,7 +187,6 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ရဂကငညဘလထအမ পরকত</t>
     </r>
@@ -174,6 +202,51 @@
   </si>
   <si>
     <t xml:space="preserve">2018-08-11T11:29:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text text text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-11T17:26:56.812+06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEN KVs test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testKV10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-11T17:26:57.812+06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO Kvs test</t>
   </si>
 </sst>
 </file>
@@ -190,7 +263,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -212,7 +284,6 @@
       <color rgb="FF000000"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -287,15 +358,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.67611336032389"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,131 +419,164 @@
       <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>27527921</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>29767031</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="P3" s="0" t="n">
         <v>123</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>456</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>3</v>
@@ -480,10 +585,10 @@
         <v>27671657</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="O4" s="1" t="n">
         <v>3</v>
@@ -491,7 +596,129 @@
       <c r="P4" s="2" t="n">
         <v>44177</v>
       </c>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="n">
+        <v>27671657</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="n">
+        <v>27671657</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Forced risk css class to lower case
</commit_message>
<xml_diff>
--- a/internewshid/chn_spreadsheet/tests/test_files/sample_kobo_keyValues.xlsx
+++ b/internewshid/chn_spreadsheet/tests/test_files/sample_kobo_keyValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -121,6 +121,9 @@
     <t xml:space="preserve">English</t>
   </si>
   <si>
+    <t xml:space="preserve">medium risk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mawkawrema </t>
   </si>
   <si>
@@ -151,6 +154,9 @@
     <t xml:space="preserve">Kutupalong RC</t>
   </si>
   <si>
+    <t xml:space="preserve">low risk</t>
+  </si>
+  <si>
     <t xml:space="preserve">553c960d-3c2f-4349-a843-742cc9495dc8</t>
   </si>
   <si>
@@ -161,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">TEN KVs test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high risk</t>
   </si>
   <si>
     <t xml:space="preserve">testKV1</t>
@@ -202,6 +211,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">tes </t>
     </r>
@@ -211,6 +221,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ရဂကငညဘလထအမ পরকত</t>
     </r>
@@ -263,6 +274,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -284,6 +296,7 @@
       <color rgb="FF000000"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -361,12 +374,12 @@
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.67611336032389"/>
   </cols>
   <sheetData>
@@ -472,20 +485,20 @@
       <c r="I2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>2</v>
+      <c r="J2" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>29767031</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>2</v>
@@ -499,44 +512,44 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>3</v>
+      <c r="J3" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="n">
         <v>27671657</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O3" s="1" t="n">
         <v>3</v>
@@ -544,118 +557,118 @@
     </row>
     <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <v>3</v>
+      <c r="J4" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>27671657</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>3</v>
+      <c r="J5" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="n">
         <v>27671657</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O5" s="1" t="n">
         <v>3</v>
@@ -664,7 +677,7 @@
         <v>44177</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -677,55 +690,55 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <v>1</v>
+      <c r="J6" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>27527921</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>